<commit_message>
Fix Modal show and close function
</commit_message>
<xml_diff>
--- a/output/materiaux_et_isolants.xlsx
+++ b/output/materiaux_et_isolants.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.04</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactorize function copy ifc file
</commit_message>
<xml_diff>
--- a/output/materiaux_et_isolants.xlsx
+++ b/output/materiaux_et_isolants.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,36 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bois</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Laine minérale</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Laine minérale</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix pattern to chose whether is a material or isolants
</commit_message>
<xml_diff>
--- a/output/materiaux_et_isolants.xlsx
+++ b/output/materiaux_et_isolants.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,32 +458,128 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Kooltherm Mousse phénolique 0.021 (0.9)_Kingspan</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Bois</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="D2" t="n">
         <v>0.012</v>
       </c>
-      <c r="C2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kooltherm Mousse phénolique 0.02 (0.9)_Kingspan</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kooltherm Mousse phénolique 0.02 (0.9)_Kingspan</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Laine minérale</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="B5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pare vapeur intérieur</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kooltherm Mousse phénolique 0.021 (0.9)_Kingspan</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Laine minérale</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>0.07000000000000001</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Laine minérale</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.04</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Myral Therm W22</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kooltherm Mousse phénolique 0.02 (0.9)_Kingspan</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kooltherm Mousse phénolique 0.02 (0.9)_Kingspan</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>